<commit_message>
Early work on room navigation and room definitions.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="87">
   <si>
     <t>Room</t>
   </si>
@@ -210,6 +210,81 @@
   </si>
   <si>
     <t>Items / Actors</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>dream</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>hall</t>
+  </si>
+  <si>
+    <t>kitchen</t>
+  </si>
+  <si>
+    <t>backyard</t>
+  </si>
+  <si>
+    <t>providence</t>
+  </si>
+  <si>
+    <t>moriarty</t>
+  </si>
+  <si>
+    <t>playground</t>
+  </si>
+  <si>
+    <t>pool</t>
+  </si>
+  <si>
+    <t>fountain</t>
+  </si>
+  <si>
+    <t>stream</t>
+  </si>
+  <si>
+    <t>livingroom</t>
+  </si>
+  <si>
+    <t>sideyard</t>
+  </si>
+  <si>
+    <t>frontyard</t>
+  </si>
+  <si>
+    <t>cornerwp</t>
+  </si>
+  <si>
+    <t>cornerwm</t>
+  </si>
+  <si>
+    <t>cornerlm</t>
+  </si>
+  <si>
+    <t>cornerlp</t>
+  </si>
+  <si>
+    <t>nearplayground</t>
+  </si>
+  <si>
+    <t>nearpool</t>
+  </si>
+  <si>
+    <t>nearfountain</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>hoodentrance</t>
+  </si>
+  <si>
+    <t>parking</t>
   </si>
 </sst>
 </file>
@@ -265,12 +340,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0148B4FE-2C22-4E89-AB56-65C8C501C9D1}" name="Table1" displayName="Table1" ref="B2:N44" totalsRowShown="0">
-  <autoFilter ref="B2:N44" xr:uid="{EE5B6242-E31E-44FE-A903-E0EDDEC89DA4}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0148B4FE-2C22-4E89-AB56-65C8C501C9D1}" name="Table1" displayName="Table1" ref="B2:O44" totalsRowShown="0">
+  <autoFilter ref="B2:O44" xr:uid="{EE5B6242-E31E-44FE-A903-E0EDDEC89DA4}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{4C79858A-8019-4F42-9CAE-DEA5B0903FF0}" name="ID"/>
     <tableColumn id="2" xr3:uid="{B19D6634-E435-4747-9D86-F5405CE79A45}" name="Room"/>
     <tableColumn id="3" xr3:uid="{C1922EF7-7251-45C0-BB4C-DBEC89BC5F91}" name="Region"/>
+    <tableColumn id="14" xr3:uid="{8376D4DF-6262-43FC-B032-DB6458AD22E2}" name="Key"/>
     <tableColumn id="11" xr3:uid="{2030DB89-9F35-40FB-A721-0E24635DEB62}" name="Percent Complete"/>
     <tableColumn id="4" xr3:uid="{B715E3E3-7417-45E4-BC99-4D841E682BC5}" name="Has Description"/>
     <tableColumn id="5" xr3:uid="{893CE564-EBD3-4573-AE21-876300DADDF4}" name="Has Nav"/>
@@ -583,27 +659,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14593EC3-B5DF-4A1E-9EFF-D51A40E025BC}">
-  <dimension ref="B2:N44"/>
+  <dimension ref="B2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -614,37 +691,40 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -654,12 +734,12 @@
       <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
       <c r="G3" t="s">
         <v>58</v>
       </c>
@@ -678,8 +758,11 @@
       <c r="L3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -689,11 +772,11 @@
       <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>58</v>
@@ -713,8 +796,11 @@
       <c r="L4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -724,11 +810,11 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
       <c r="G5" t="s">
         <v>58</v>
@@ -748,8 +834,11 @@
       <c r="L5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -759,11 +848,11 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6" t="s">
         <v>58</v>
@@ -783,8 +872,11 @@
       <c r="L6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>5</v>
       </c>
@@ -794,11 +886,11 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
       <c r="G7" t="s">
         <v>58</v>
@@ -818,8 +910,11 @@
       <c r="L7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -829,11 +924,11 @@
       <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>58</v>
@@ -853,8 +948,11 @@
       <c r="L8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>7</v>
       </c>
@@ -864,11 +962,11 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
+      <c r="E9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
       </c>
       <c r="G9" t="s">
         <v>58</v>
@@ -888,8 +986,11 @@
       <c r="L9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>8</v>
       </c>
@@ -899,11 +1000,11 @@
       <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>58</v>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
       </c>
       <c r="G10" t="s">
         <v>58</v>
@@ -923,8 +1024,11 @@
       <c r="L10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>9</v>
       </c>
@@ -934,11 +1038,11 @@
       <c r="D11" t="s">
         <v>11</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>58</v>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11" t="s">
         <v>58</v>
@@ -958,8 +1062,11 @@
       <c r="L11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -969,11 +1076,11 @@
       <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
-        <v>58</v>
+      <c r="E12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
       </c>
       <c r="G12" t="s">
         <v>58</v>
@@ -993,8 +1100,11 @@
       <c r="L12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>11</v>
       </c>
@@ -1004,11 +1114,11 @@
       <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>58</v>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
       <c r="G13" t="s">
         <v>58</v>
@@ -1028,8 +1138,11 @@
       <c r="L13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>12</v>
       </c>
@@ -1039,11 +1152,11 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
       </c>
       <c r="G14" t="s">
         <v>58</v>
@@ -1063,8 +1176,11 @@
       <c r="L14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>13</v>
       </c>
@@ -1074,11 +1190,11 @@
       <c r="D15" t="s">
         <v>11</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
-        <v>58</v>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
       <c r="G15" t="s">
         <v>58</v>
@@ -1098,8 +1214,11 @@
       <c r="L15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14</v>
       </c>
@@ -1109,11 +1228,11 @@
       <c r="D16" t="s">
         <v>11</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
-        <v>58</v>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
       </c>
       <c r="G16" t="s">
         <v>58</v>
@@ -1133,8 +1252,11 @@
       <c r="L16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
@@ -1144,11 +1266,11 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
-        <v>58</v>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
       </c>
       <c r="G17" t="s">
         <v>58</v>
@@ -1168,8 +1290,11 @@
       <c r="L17" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>16</v>
       </c>
@@ -1179,11 +1304,11 @@
       <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
-        <v>58</v>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
       <c r="G18" t="s">
         <v>58</v>
@@ -1203,8 +1328,11 @@
       <c r="L18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>17</v>
       </c>
@@ -1214,11 +1342,11 @@
       <c r="D19" t="s">
         <v>11</v>
       </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
       </c>
       <c r="G19" t="s">
         <v>58</v>
@@ -1238,8 +1366,11 @@
       <c r="L19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>18</v>
       </c>
@@ -1249,11 +1380,11 @@
       <c r="D20" t="s">
         <v>11</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>58</v>
+      <c r="E20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
       <c r="G20" t="s">
         <v>58</v>
@@ -1273,8 +1404,11 @@
       <c r="L20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>19</v>
       </c>
@@ -1284,11 +1418,11 @@
       <c r="D21" t="s">
         <v>11</v>
       </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
+      <c r="E21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
       </c>
       <c r="G21" t="s">
         <v>58</v>
@@ -1308,8 +1442,11 @@
       <c r="L21" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>20</v>
       </c>
@@ -1319,11 +1456,11 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
-        <v>58</v>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
       </c>
       <c r="G22" t="s">
         <v>58</v>
@@ -1343,8 +1480,11 @@
       <c r="L22" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>21</v>
       </c>
@@ -1354,11 +1494,11 @@
       <c r="D23" t="s">
         <v>11</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
-        <v>58</v>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
       </c>
       <c r="G23" t="s">
         <v>58</v>
@@ -1378,8 +1518,11 @@
       <c r="L23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>22</v>
       </c>
@@ -1389,11 +1532,11 @@
       <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
       </c>
       <c r="G24" t="s">
         <v>58</v>
@@ -1413,8 +1556,11 @@
       <c r="L24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>23</v>
       </c>
@@ -1424,11 +1570,8 @@
       <c r="D25" t="s">
         <v>44</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
-        <v>58</v>
+      <c r="F25">
+        <v>0</v>
       </c>
       <c r="G25" t="s">
         <v>58</v>
@@ -1448,8 +1591,11 @@
       <c r="L25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>24</v>
       </c>
@@ -1459,11 +1605,8 @@
       <c r="D26" t="s">
         <v>44</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
-        <v>58</v>
+      <c r="F26">
+        <v>0</v>
       </c>
       <c r="G26" t="s">
         <v>58</v>
@@ -1483,8 +1626,11 @@
       <c r="L26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>25</v>
       </c>
@@ -1494,11 +1640,8 @@
       <c r="D27" t="s">
         <v>44</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
+      <c r="F27">
+        <v>0</v>
       </c>
       <c r="G27" t="s">
         <v>58</v>
@@ -1518,8 +1661,11 @@
       <c r="L27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>26</v>
       </c>
@@ -1529,11 +1675,8 @@
       <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
-        <v>58</v>
+      <c r="F28">
+        <v>0</v>
       </c>
       <c r="G28" t="s">
         <v>58</v>
@@ -1553,8 +1696,11 @@
       <c r="L28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>27</v>
       </c>
@@ -1564,11 +1710,8 @@
       <c r="D29" t="s">
         <v>43</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
-        <v>58</v>
+      <c r="F29">
+        <v>0</v>
       </c>
       <c r="G29" t="s">
         <v>58</v>
@@ -1588,8 +1731,11 @@
       <c r="L29" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>28</v>
       </c>
@@ -1599,11 +1745,8 @@
       <c r="D30" t="s">
         <v>43</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
-        <v>58</v>
+      <c r="F30">
+        <v>0</v>
       </c>
       <c r="G30" t="s">
         <v>58</v>
@@ -1623,8 +1766,11 @@
       <c r="L30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>29</v>
       </c>
@@ -1634,11 +1780,8 @@
       <c r="D31" t="s">
         <v>43</v>
       </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>58</v>
+      <c r="F31">
+        <v>0</v>
       </c>
       <c r="G31" t="s">
         <v>58</v>
@@ -1658,8 +1801,11 @@
       <c r="L31" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>30</v>
       </c>
@@ -1669,11 +1815,8 @@
       <c r="D32" t="s">
         <v>43</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32" t="s">
-        <v>58</v>
+      <c r="F32">
+        <v>0</v>
       </c>
       <c r="G32" t="s">
         <v>58</v>
@@ -1693,8 +1836,11 @@
       <c r="L32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>31</v>
       </c>
@@ -1704,11 +1850,11 @@
       <c r="D33" t="s">
         <v>56</v>
       </c>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>58</v>
+      <c r="E33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
       </c>
       <c r="G33" t="s">
         <v>58</v>
@@ -1728,8 +1874,11 @@
       <c r="L33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>32</v>
       </c>
@@ -1739,11 +1888,8 @@
       <c r="D34" t="s">
         <v>56</v>
       </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>58</v>
+      <c r="F34">
+        <v>0</v>
       </c>
       <c r="G34" t="s">
         <v>58</v>
@@ -1763,8 +1909,11 @@
       <c r="L34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>33</v>
       </c>
@@ -1774,11 +1923,8 @@
       <c r="D35" t="s">
         <v>56</v>
       </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>58</v>
+      <c r="F35">
+        <v>0</v>
       </c>
       <c r="G35" t="s">
         <v>58</v>
@@ -1798,8 +1944,11 @@
       <c r="L35" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>34</v>
       </c>
@@ -1809,11 +1958,8 @@
       <c r="D36" t="s">
         <v>56</v>
       </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>58</v>
+      <c r="F36">
+        <v>0</v>
       </c>
       <c r="G36" t="s">
         <v>58</v>
@@ -1833,8 +1979,11 @@
       <c r="L36" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>35</v>
       </c>
@@ -1844,11 +1993,8 @@
       <c r="D37" t="s">
         <v>56</v>
       </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="s">
-        <v>58</v>
+      <c r="F37">
+        <v>0</v>
       </c>
       <c r="G37" t="s">
         <v>58</v>
@@ -1868,8 +2014,11 @@
       <c r="L37" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>36</v>
       </c>
@@ -1879,11 +2028,8 @@
       <c r="D38" t="s">
         <v>56</v>
       </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38" t="s">
-        <v>58</v>
+      <c r="F38">
+        <v>0</v>
       </c>
       <c r="G38" t="s">
         <v>58</v>
@@ -1903,8 +2049,11 @@
       <c r="L38" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>37</v>
       </c>
@@ -1914,11 +2063,8 @@
       <c r="D39" t="s">
         <v>56</v>
       </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39" t="s">
-        <v>58</v>
+      <c r="F39">
+        <v>0</v>
       </c>
       <c r="G39" t="s">
         <v>58</v>
@@ -1938,8 +2084,11 @@
       <c r="L39" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>38</v>
       </c>
@@ -1949,11 +2098,8 @@
       <c r="D40" t="s">
         <v>56</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40" t="s">
-        <v>58</v>
+      <c r="F40">
+        <v>0</v>
       </c>
       <c r="G40" t="s">
         <v>58</v>
@@ -1973,8 +2119,11 @@
       <c r="L40" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>39</v>
       </c>
@@ -1984,11 +2133,8 @@
       <c r="D41" t="s">
         <v>56</v>
       </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41" t="s">
-        <v>58</v>
+      <c r="F41">
+        <v>0</v>
       </c>
       <c r="G41" t="s">
         <v>58</v>
@@ -2008,8 +2154,11 @@
       <c r="L41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>40</v>
       </c>
@@ -2019,11 +2168,8 @@
       <c r="D42" t="s">
         <v>56</v>
       </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" t="s">
-        <v>58</v>
+      <c r="F42">
+        <v>0</v>
       </c>
       <c r="G42" t="s">
         <v>58</v>
@@ -2043,8 +2189,11 @@
       <c r="L42" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>41</v>
       </c>
@@ -2054,11 +2203,8 @@
       <c r="D43" t="s">
         <v>56</v>
       </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43" t="s">
-        <v>58</v>
+      <c r="F43">
+        <v>0</v>
       </c>
       <c r="G43" t="s">
         <v>58</v>
@@ -2078,8 +2224,11 @@
       <c r="L43" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>42</v>
       </c>
@@ -2089,11 +2238,11 @@
       <c r="D44" t="s">
         <v>11</v>
       </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44" t="s">
-        <v>58</v>
+      <c r="E44" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
       </c>
       <c r="G44" t="s">
         <v>58</v>
@@ -2111,13 +2260,17 @@
         <v>58</v>
       </c>
       <c r="L44" t="s">
+        <v>58</v>
+      </c>
+      <c r="M44" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Re-ordered some design files. Expanded room connections.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\angularIF\design\Fog Terrier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\angularIF\design\Fog Terrier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{8095B8DC-B90B-44CF-8709-1A4BE289C517}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="88">
   <si>
     <t>Room</t>
   </si>
@@ -285,12 +285,15 @@
   </si>
   <si>
     <t>parking</t>
+  </si>
+  <si>
+    <t>trail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,23 +343,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0148B4FE-2C22-4E89-AB56-65C8C501C9D1}" name="Table1" displayName="Table1" ref="B2:O44" totalsRowShown="0">
-  <autoFilter ref="B2:O44" xr:uid="{EE5B6242-E31E-44FE-A903-E0EDDEC89DA4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:O44" totalsRowShown="0">
+  <autoFilter ref="B2:O44"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{4C79858A-8019-4F42-9CAE-DEA5B0903FF0}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{B19D6634-E435-4747-9D86-F5405CE79A45}" name="Room"/>
-    <tableColumn id="3" xr3:uid="{C1922EF7-7251-45C0-BB4C-DBEC89BC5F91}" name="Region"/>
-    <tableColumn id="14" xr3:uid="{8376D4DF-6262-43FC-B032-DB6458AD22E2}" name="Key"/>
-    <tableColumn id="11" xr3:uid="{2030DB89-9F35-40FB-A721-0E24635DEB62}" name="Percent Complete"/>
-    <tableColumn id="4" xr3:uid="{B715E3E3-7417-45E4-BC99-4D841E682BC5}" name="Has Description"/>
-    <tableColumn id="5" xr3:uid="{893CE564-EBD3-4573-AE21-876300DADDF4}" name="Has Nav"/>
-    <tableColumn id="6" xr3:uid="{2091BE54-7770-4C20-90C0-132560F6079E}" name="Has Objects"/>
-    <tableColumn id="7" xr3:uid="{773FE17F-BFE5-43D6-B415-63DFA8C59EED}" name="Has Tests"/>
-    <tableColumn id="8" xr3:uid="{D1E4535B-D454-4770-AEFF-BB852C1B9173}" name="Has Atmospherics"/>
-    <tableColumn id="9" xr3:uid="{6A3D999D-4C41-4442-A3F1-900104999F2E}" name="Has Verbs"/>
-    <tableColumn id="10" xr3:uid="{0716AF9B-9E85-4C71-B824-711B92CECD00}" name="Has Aliases"/>
-    <tableColumn id="12" xr3:uid="{AB285F2F-D74D-4ABC-BF73-BB3215CB7037}" name="Objects"/>
-    <tableColumn id="13" xr3:uid="{B9FF1466-6A75-416F-887E-F0AF8FA0AE1E}" name="Items / Actors"/>
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Room"/>
+    <tableColumn id="3" name="Region"/>
+    <tableColumn id="14" name="Key"/>
+    <tableColumn id="11" name="Percent Complete"/>
+    <tableColumn id="4" name="Has Description"/>
+    <tableColumn id="5" name="Has Nav"/>
+    <tableColumn id="6" name="Has Objects"/>
+    <tableColumn id="7" name="Has Tests"/>
+    <tableColumn id="8" name="Has Atmospherics"/>
+    <tableColumn id="9" name="Has Verbs"/>
+    <tableColumn id="10" name="Has Aliases"/>
+    <tableColumn id="12" name="Objects"/>
+    <tableColumn id="13" name="Items / Actors"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,11 +661,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14593EC3-B5DF-4A1E-9EFF-D51A40E025BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,6 +1818,9 @@
       <c r="D32" t="s">
         <v>43</v>
       </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
       <c r="F32">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated UI. Added first room description.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\angularIF\design\Fog Terrier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\angularIF\design\Fog Terrier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,25 +472,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:N44" totalsRowShown="0">
-  <autoFilter ref="B2:N44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B2:N44" totalsRowShown="0">
+  <autoFilter ref="B2:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="B3:N44">
     <sortCondition ref="D2:D44"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="14" name="Key"/>
-    <tableColumn id="2" name="Room"/>
-    <tableColumn id="3" name="Region"/>
-    <tableColumn id="11" name="Percent Complete"/>
-    <tableColumn id="5" name="Has Nav"/>
-    <tableColumn id="4" name="Has Description"/>
-    <tableColumn id="6" name="Num Objects"/>
-    <tableColumn id="8" name="Num Atmospherics"/>
-    <tableColumn id="9" name="Num Verbs"/>
-    <tableColumn id="10" name="Num Aliases"/>
-    <tableColumn id="7" name="Num Tests"/>
-    <tableColumn id="12" name="Objects"/>
-    <tableColumn id="13" name="Items / Actors"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Key"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Room"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Region"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Percent Complete"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Has Nav"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Has Description"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Num Objects"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Num Atmospherics"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Num Verbs"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Num Aliases"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Num Tests"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Objects"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Items / Actors"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -792,11 +792,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>

</xml_diff>

<commit_message>
#380, #431 - Added story content.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -866,7 +866,7 @@
   <dimension ref="B2:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,13 +1499,13 @@
         <v>5</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1604,13 +1604,13 @@
         <v>5</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1639,13 +1639,13 @@
         <v>5</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="E45" s="7">
         <f>SUM(Table1[Percent Complete])/(COUNT(Table1[Percent Complete])*100)</f>
-        <v>1.4285714285714285E-2</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="F45" s="8">
         <f>SUM(Table1[Has Nav])/COUNT(Table1[Has Nav])</f>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="G45" s="8">
         <f>SUM(Table1[Has Description])/COUNT(Table1[Has Description])</f>
-        <v>0.16666666666666666</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="H45">
         <f>SUBTOTAL(109,Table1[Num Objects])</f>

</xml_diff>

<commit_message>
Updated content. 60% done with descriptions.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -866,7 +866,7 @@
   <dimension ref="B2:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,13 +974,13 @@
         <v>37</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -1009,13 +1009,13 @@
         <v>37</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1044,13 +1044,13 @@
         <v>37</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1184,7 +1184,7 @@
         <v>21</v>
       </c>
       <c r="E10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1254,13 +1254,13 @@
         <v>21</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2404,7 +2404,7 @@
       </c>
       <c r="E45" s="7">
         <f>SUM(Table1[Percent Complete])/(COUNT(Table1[Percent Complete])*100)</f>
-        <v>5.1190476190476189E-2</v>
+        <v>6.5476190476190479E-2</v>
       </c>
       <c r="F45" s="8">
         <f>SUM(Table1[Has Nav])/COUNT(Table1[Has Nav])</f>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="G45" s="8">
         <f>SUM(Table1[Has Description])/COUNT(Table1[Has Description])</f>
-        <v>0.5</v>
+        <v>0.59523809523809523</v>
       </c>
       <c r="H45">
         <f>SUBTOTAL(109,Table1[Num Objects])</f>

</xml_diff>

<commit_message>
Auto stash before merge of "develop" and "GitLab/develop"
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -865,7 +865,7 @@
   <dimension ref="B2:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,13 +2198,13 @@
         <v>46</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="E45" s="7">
         <f>SUM(Table1[Percent Complete])/(COUNT(Table1[Percent Complete])*100)</f>
-        <v>9.6428571428571433E-2</v>
+        <v>9.8809523809523805E-2</v>
       </c>
       <c r="F45" s="8">
         <f>SUM(Table1[Has Nav])/COUNT(Table1[Has Nav])</f>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="G45" s="8">
         <f>SUM(Table1[Has Description])/COUNT(Table1[Has Description])</f>
-        <v>0.90476190476190477</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="H45">
         <f>SUBTOTAL(109,Table1[Num Objects])</f>

</xml_diff>

<commit_message>
Editor usability improvements; starting to define story content.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\angularIF\design\Fog Terrier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\angularIF\design\Fog Terrier\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,31 +535,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:N45" totalsRowCount="1">
-  <autoFilter ref="B2:N44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B2:N45" totalsRowCount="1">
+  <autoFilter ref="B2:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="B3:N44">
     <sortCondition ref="D2:D44"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="14" name="Key" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Room"/>
-    <tableColumn id="3" name="Region"/>
-    <tableColumn id="11" name="Percent Complete" totalsRowFunction="custom" totalsRowDxfId="2">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Key" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Room"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Region"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Percent Complete" totalsRowFunction="custom" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Table1[Percent Complete])/(COUNT(Table1[Percent Complete])*100)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Has Nav" totalsRowFunction="custom" totalsRowDxfId="1">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Has Nav" totalsRowFunction="custom" totalsRowDxfId="1">
       <totalsRowFormula>SUM(Table1[Has Nav])/COUNT(Table1[Has Nav])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Has Description" totalsRowFunction="custom" totalsRowDxfId="0">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Has Description" totalsRowFunction="custom" totalsRowDxfId="0">
       <totalsRowFormula>SUM(Table1[Has Description])/COUNT(Table1[Has Description])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Num Objects" totalsRowFunction="sum"/>
-    <tableColumn id="8" name="Num Atmospherics" totalsRowFunction="sum"/>
-    <tableColumn id="9" name="Num Verbs" totalsRowFunction="sum"/>
-    <tableColumn id="10" name="Num Aliases" totalsRowFunction="sum"/>
-    <tableColumn id="7" name="Num Tests" totalsRowFunction="sum"/>
-    <tableColumn id="12" name="Objects"/>
-    <tableColumn id="13" name="Items / Actors" totalsRowFunction="count"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Num Objects" totalsRowFunction="sum"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Num Atmospherics" totalsRowFunction="sum"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Num Verbs" totalsRowFunction="sum"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Num Aliases" totalsRowFunction="sum"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Num Tests" totalsRowFunction="sum"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Objects"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Items / Actors" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -861,11 +861,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1157,7 +1157,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1227,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1367,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1402,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1647,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="H45">
         <f>SUBTOTAL(109,Table1[Num Objects])</f>
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="I45">
         <f>SUBTOTAL(109,Table1[Num Atmospherics])</f>
@@ -2440,7 +2440,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F45:G45">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2454,7 +2454,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E44 E46:E1048576">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -2468,7 +2468,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2477,6 +2477,20 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{47F17CD7-98A0-402E-8EF5-B3891CF47ABA}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H44">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFB628"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0FC7FA8A-53D9-4A9C-B8DC-BF504B655AA3}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2531,7 +2545,7 @@
           <xm:sqref>E45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="10" id="{52AA128E-9E5C-4D26-A1FB-1AB3B1EFA284}">
+          <x14:cfRule type="iconSet" priority="11" id="{52AA128E-9E5C-4D26-A1FB-1AB3B1EFA284}">
             <x14:iconSet iconSet="3Symbols" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -2549,6 +2563,17 @@
           </x14:cfRule>
           <xm:sqref>F3:G44</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0FC7FA8A-53D9-4A9C-B8DC-BF504B655AA3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:H44</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Progress on story content
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1822,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="H45">
         <f>SUBTOTAL(109,Table1[Num Objects])</f>
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="I45">
         <f>SUBTOTAL(109,Table1[Num Atmospherics])</f>

</xml_diff>

<commit_message>
Content. Coming along nicely.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1472,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1507,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -1542,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1577,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1682,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="H45">
         <f>SUBTOTAL(109,Table1[Num Objects])</f>
-        <v>132</v>
+        <v>213</v>
       </c>
       <c r="I45">
         <f>SUBTOTAL(109,Table1[Num Atmospherics])</f>
@@ -2545,6 +2545,17 @@
           <xm:sqref>E45</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0FC7FA8A-53D9-4A9C-B8DC-BF504B655AA3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H3:H44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="11" id="{52AA128E-9E5C-4D26-A1FB-1AB3B1EFA284}">
             <x14:iconSet iconSet="3Symbols" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -2563,17 +2574,6 @@
           </x14:cfRule>
           <xm:sqref>F3:G44</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0FC7FA8A-53D9-4A9C-B8DC-BF504B655AA3}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>H3:H44</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Getting unit tests online. Slowly.
</commit_message>
<xml_diff>
--- a/design/Fog Terrier/Status.xlsx
+++ b/design/Fog Terrier/Status.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Backdrop Objects" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="136">
   <si>
     <t>Room</t>
   </si>
@@ -337,6 +338,102 @@
   </si>
   <si>
     <t>Overgrown Trail</t>
+  </si>
+  <si>
+    <t>Unique Objects</t>
+  </si>
+  <si>
+    <t>Fog</t>
+  </si>
+  <si>
+    <t>Mist</t>
+  </si>
+  <si>
+    <t>Lebling Drive</t>
+  </si>
+  <si>
+    <t>Anderson Science Center</t>
+  </si>
+  <si>
+    <t>Anderson Science Center Internal Lighting (from outside)</t>
+  </si>
+  <si>
+    <t>College</t>
+  </si>
+  <si>
+    <t>Pond</t>
+  </si>
+  <si>
+    <t>Algae</t>
+  </si>
+  <si>
+    <t>Fountains (Pond Fountains)</t>
+  </si>
+  <si>
+    <t>Warmer Air</t>
+  </si>
+  <si>
+    <t>Pond Water</t>
+  </si>
+  <si>
+    <t>Condos</t>
+  </si>
+  <si>
+    <t>Apartments</t>
+  </si>
+  <si>
+    <t>Whateley Drive</t>
+  </si>
+  <si>
+    <t>Streetlights</t>
+  </si>
+  <si>
+    <t>Your House</t>
+  </si>
+  <si>
+    <t>Vacant Houses</t>
+  </si>
+  <si>
+    <t>Neighboring Houses</t>
+  </si>
+  <si>
+    <t>Sidewalk</t>
+  </si>
+  <si>
+    <t>Darkness</t>
+  </si>
+  <si>
+    <t>Exercise Equipment</t>
+  </si>
+  <si>
+    <t>Breeze</t>
+  </si>
+  <si>
+    <t>Ravenwood Avenue (Main Road)</t>
+  </si>
+  <si>
+    <t>Grassy Field</t>
+  </si>
+  <si>
+    <t>Tall Grass</t>
+  </si>
+  <si>
+    <t>Leaves</t>
+  </si>
+  <si>
+    <t>Interior Walls</t>
+  </si>
+  <si>
+    <t>Carpet</t>
+  </si>
+  <si>
+    <t>Weed Whacker</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -535,12 +632,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B2:N45" totalsRowCount="1">
-  <autoFilter ref="B2:N44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="B3:N44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B2:O45" totalsRowCount="1">
+  <autoFilter ref="B2:O44" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="B3:O44">
     <sortCondition ref="D2:D44"/>
   </sortState>
-  <tableColumns count="13">
+  <tableColumns count="14">
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Key" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Room"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Region"/>
@@ -554,6 +651,7 @@
       <totalsRowFormula>SUM(Table1[Has Description])/COUNT(Table1[Has Description])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Num Objects" totalsRowFunction="sum"/>
+    <tableColumn id="1" xr3:uid="{1F3F3064-EB29-4DDB-8AB6-782E25314AEA}" name="Unique Objects" totalsRowFunction="sum"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Num Atmospherics" totalsRowFunction="sum"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Num Verbs" totalsRowFunction="sum"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Num Aliases" totalsRowFunction="sum"/>
@@ -562,6 +660,16 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Items / Actors" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{370F0FB4-96E2-4C46-B489-0CA01925692F}" name="Table2" displayName="Table2" ref="B2:B37" totalsRowShown="0">
+  <autoFilter ref="B2:B37" xr:uid="{8401ADF9-232B-486F-9709-95909D643E99}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{80367FD4-404F-4F37-BCE8-D690C0FBA9E9}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -862,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N45"/>
+  <dimension ref="B2:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,17 +984,18 @@
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>49</v>
       </c>
@@ -909,25 +1018,28 @@
         <v>96</v>
       </c>
       <c r="I2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" t="s">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>94</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>93</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>92</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>50</v>
       </c>
@@ -950,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -961,8 +1073,11 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>60</v>
       </c>
@@ -985,7 +1100,7 @@
         <v>6</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -996,8 +1111,11 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>76</v>
       </c>
@@ -1020,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1031,8 +1149,11 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>77</v>
       </c>
@@ -1055,7 +1176,7 @@
         <v>3</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1066,8 +1187,11 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>78</v>
       </c>
@@ -1090,7 +1214,7 @@
         <v>10</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1101,8 +1225,11 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>83</v>
       </c>
@@ -1125,7 +1252,7 @@
         <v>6</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1136,8 +1263,11 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>51</v>
       </c>
@@ -1160,7 +1290,7 @@
         <v>7</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1171,8 +1301,11 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -1195,7 +1328,7 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1206,8 +1339,11 @@
       <c r="L10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -1230,7 +1366,7 @@
         <v>10</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1241,8 +1377,11 @@
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -1265,7 +1404,7 @@
         <v>9</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1276,8 +1415,11 @@
       <c r="L12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>54</v>
       </c>
@@ -1300,7 +1442,7 @@
         <v>9</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1311,8 +1453,11 @@
       <c r="L13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>62</v>
       </c>
@@ -1335,7 +1480,7 @@
         <v>11</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1346,8 +1491,11 @@
       <c r="L14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>63</v>
       </c>
@@ -1370,7 +1518,7 @@
         <v>16</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1381,8 +1529,11 @@
       <c r="L15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>64</v>
       </c>
@@ -1405,7 +1556,7 @@
         <v>8</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1416,8 +1567,11 @@
       <c r="L16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>68</v>
       </c>
@@ -1440,7 +1594,7 @@
         <v>8</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1451,8 +1605,11 @@
       <c r="L17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>65</v>
       </c>
@@ -1475,7 +1632,7 @@
         <v>6</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1486,8 +1643,11 @@
       <c r="L18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>57</v>
       </c>
@@ -1510,7 +1670,7 @@
         <v>11</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1521,8 +1681,11 @@
       <c r="L19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>56</v>
       </c>
@@ -1545,7 +1708,7 @@
         <v>7</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1556,8 +1719,11 @@
       <c r="L20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>66</v>
       </c>
@@ -1591,8 +1757,11 @@
       <c r="L21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>71</v>
       </c>
@@ -1615,7 +1784,7 @@
         <v>12</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1626,8 +1795,11 @@
       <c r="L22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>58</v>
       </c>
@@ -1650,7 +1822,7 @@
         <v>17</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1661,8 +1833,11 @@
       <c r="L23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>69</v>
       </c>
@@ -1685,7 +1860,7 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1696,8 +1871,11 @@
       <c r="L24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>70</v>
       </c>
@@ -1720,7 +1898,7 @@
         <v>6</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1731,8 +1909,11 @@
       <c r="L25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>67</v>
       </c>
@@ -1755,7 +1936,7 @@
         <v>8</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1766,8 +1947,11 @@
       <c r="L26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>55</v>
       </c>
@@ -1790,7 +1974,7 @@
         <v>5</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1801,8 +1985,11 @@
       <c r="L27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -1825,7 +2012,7 @@
         <v>7</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -1836,8 +2023,11 @@
       <c r="L28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>72</v>
       </c>
@@ -1860,7 +2050,7 @@
         <v>10</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1871,8 +2061,11 @@
       <c r="L29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>100</v>
       </c>
@@ -1895,7 +2088,7 @@
         <v>11</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1906,8 +2099,11 @@
       <c r="L30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>73</v>
       </c>
@@ -1930,7 +2126,7 @@
         <v>9</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -1941,8 +2137,11 @@
       <c r="L31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -1965,7 +2164,7 @@
         <v>9</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -1976,8 +2175,11 @@
       <c r="L32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>87</v>
       </c>
@@ -2000,7 +2202,7 @@
         <v>8</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -2011,8 +2213,11 @@
       <c r="L33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>88</v>
       </c>
@@ -2035,7 +2240,7 @@
         <v>9</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -2046,8 +2251,11 @@
       <c r="L34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>89</v>
       </c>
@@ -2070,7 +2278,7 @@
         <v>6</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -2081,8 +2289,11 @@
       <c r="L35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -2105,7 +2316,7 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2116,8 +2327,11 @@
       <c r="L36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>85</v>
       </c>
@@ -2140,7 +2354,7 @@
         <v>5</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -2151,8 +2365,11 @@
       <c r="L37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>90</v>
       </c>
@@ -2175,7 +2392,7 @@
         <v>8</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2186,8 +2403,11 @@
       <c r="L38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>86</v>
       </c>
@@ -2210,7 +2430,7 @@
         <v>9</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2221,8 +2441,11 @@
       <c r="L39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>91</v>
       </c>
@@ -2245,7 +2468,7 @@
         <v>10</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2256,8 +2479,11 @@
       <c r="L40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>80</v>
       </c>
@@ -2280,7 +2506,7 @@
         <v>6</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2291,8 +2517,11 @@
       <c r="L41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>81</v>
       </c>
@@ -2315,7 +2544,7 @@
         <v>8</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -2326,8 +2555,11 @@
       <c r="L42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>82</v>
       </c>
@@ -2350,7 +2582,7 @@
         <v>8</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2361,8 +2593,11 @@
       <c r="L43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>74</v>
       </c>
@@ -2385,7 +2620,7 @@
         <v>8</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -2396,8 +2631,11 @@
       <c r="L44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>97</v>
       </c>
@@ -2418,22 +2656,26 @@
         <v>353</v>
       </c>
       <c r="I45">
+        <f>SUBTOTAL(109,Table1[Unique Objects])</f>
+        <v>252</v>
+      </c>
+      <c r="J45">
         <f>SUBTOTAL(109,Table1[Num Atmospherics])</f>
         <v>0</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <f>SUBTOTAL(109,Table1[Num Verbs])</f>
         <v>0</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <f>SUBTOTAL(109,Table1[Num Aliases])</f>
         <v>0</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <f>SUBTOTAL(109,Table1[Num Tests])</f>
         <v>0</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <f>SUBTOTAL(103,Table1[Items / Actors])</f>
         <v>0</v>
       </c>
@@ -2481,7 +2723,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H44">
+  <conditionalFormatting sqref="H3:I44">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2553,7 +2795,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H3:H44</xm:sqref>
+          <xm:sqref>H3:I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="11" id="{52AA128E-9E5C-4D26-A1FB-1AB3B1EFA284}">
@@ -2578,4 +2820,206 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A02092-67D6-462E-909B-2C6A4E9FBE82}">
+  <dimension ref="B2:B37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>